<commit_message>
Added Logout and Forgot Password test cases to Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/Test_Cases/Test Cases.xlsx
+++ b/Test_Cases/Test Cases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\SQA Projects\OpenCart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OpenCart_SQA_Project_2025\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="464">
   <si>
     <t>Project Name</t>
   </si>
@@ -369,9 +369,6 @@
   </si>
   <si>
     <t>Verify special characters in Email</t>
-  </si>
-  <si>
-    <t>name#email.com</t>
   </si>
   <si>
     <t>Verify redirection after successful registration</t>
@@ -544,12 +541,6 @@
   </si>
   <si>
     <t>TC_REG_026</t>
-  </si>
-  <si>
-    <t>First Name: Muhammad
-Last Name: Usman
-Email: usman@gmail.com
-Password: test123</t>
   </si>
   <si>
     <t>1. Navigate to Homepage
@@ -566,9 +557,6 @@
 5. Click on "Submit" button.</t>
   </si>
   <si>
-    <t>Email: usman@gmail.com</t>
-  </si>
-  <si>
     <t>1. Navigate to Homepage
 2. Click on "My Account" dropdown in Header
 3. Click on "Register" from the dropdown
@@ -594,13 +582,6 @@
 3. Click on "Register" from the dropdown
 4. Leave last name empty 
 5. Click on "Submit" button</t>
-  </si>
-  <si>
-    <t>abc@gmail / abc@g.com</t>
-  </si>
-  <si>
-    <t>Numbers/special chars in name
-Muh@mmad</t>
   </si>
   <si>
     <t>1. Navigate to Homepage
@@ -882,12 +863,6 @@
     <t>Tester must have DB access (via phpMyAdmin)</t>
   </si>
   <si>
-    <t>First Name: Usman
-Last Name: Ali
-Email: usmanali@example.com
-Password: Test@1234</t>
-  </si>
-  <si>
     <t>1. Click on 'My Account' in the header
 2. Click on 'Register'
 3. Enter valid details in all fields
@@ -1094,12 +1069,6 @@
 Password: validPassword</t>
   </si>
   <si>
-    <t>Email: test@example.comPassword: validPassword</t>
-  </si>
-  <si>
-    <t>User is on the Login page</t>
-  </si>
-  <si>
     <t>Verify password field hides input</t>
   </si>
   <si>
@@ -1115,18 +1084,9 @@
     <t>User is logged in</t>
   </si>
   <si>
-    <t>Verify error for invalid email format</t>
-  </si>
-  <si>
-    <t>Error: "Invalid email format"</t>
-  </si>
-  <si>
     <t>Verify Login page accessible from other pages</t>
   </si>
   <si>
-    <t>Should show placeholders like "E-Mail Address", "Password"</t>
-  </si>
-  <si>
     <t>Verify mobile responsiveness</t>
   </si>
   <si>
@@ -1137,18 +1097,6 @@
   </si>
   <si>
     <t>Properly displayed layout</t>
-  </si>
-  <si>
-    <t>Redirect to originally requested page</t>
-  </si>
-  <si>
-    <t>Verify that the login form fields have appropriate placeholder text</t>
-  </si>
-  <si>
-    <t>1. Navigate to Homepage
-2. Click on "My Account" dropdown in Header
-3. Click on "Login" from the dropdown
-4. Inspect the Email and Password fields</t>
   </si>
   <si>
     <t>User should be logged in successfully</t>
@@ -1198,13 +1146,6 @@
 3. Click on "Login" from the dropdown
 4. Enter the valid email in uppercase and the valid password
 5. Click on "Login" button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Navigate to Homepage
-2. Click on "My Account" dropdown in Header
-3. Click on "Login" from the dropdown
-4. Enter invalid email format
-5. Click on "Login" button </t>
   </si>
   <si>
     <t>Email: invalidEmail
@@ -1325,6 +1266,502 @@
   <si>
     <t>1. User should remain logged in
 2. "My Account" dropdown should display Logout, Order History, etc.</t>
+  </si>
+  <si>
+    <t>Verify account is temporarily locked after multiple failed login attempts</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage
+2. Click on "My Account" dropdown in Header
+3. Click on "Login" from the dropdown
+4. Enter invalid Email and Password
+5. Click on "Login" button
+6. Repeat steps 4–5 a total of 5 times</t>
+  </si>
+  <si>
+    <t>1. On the 5th attempt, an error should be displayed:
+"Warning: Your account has exceeded allowed number of login attempts. Please try again in 1 hour</t>
+  </si>
+  <si>
+    <t>Verify UI layout and design consistency on Login page</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage
+2. Click on "My Account" dropdown in Header
+3. Click on "Login" from the dropdown
+4. Observe the overall layout of the Login page including:
+- Alignment of Email and Password fields
+- Size and position of “Login” and “Forgotten Password” buttons
+- Visibility and spelling of all labels and placeholders
+- Spacing and padding around fields and sections</t>
+  </si>
+  <si>
+    <t>1. All UI elements should be properly aligned
+2. Buttons should be uniform in size and easily clickable
+3. Labels and placeholders should be clearly visible and free of typos
+4. Page should appear clean and consistently spaced</t>
+  </si>
+  <si>
+    <t>Verify login using keyboard navigation (Tab and Enter keys)</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage
+2. Click on "My Account" dropdown in Header
+3. Click on "Login" from the dropdown
+4. Press Tab key until the cursor focuses on "E-Mail Address" field
+5. Enter valid Email
+6. Press Tab to move to "Password" field
+7. Enter valid Password
+8. Press Tab to highlight "Login" button
+9. Press Enter key to submit</t>
+  </si>
+  <si>
+    <t>1. User should be logged in successfully and redirected to My Account page</t>
+  </si>
+  <si>
+    <t>Email: test@example.com</t>
+  </si>
+  <si>
+    <t>test#example.com</t>
+  </si>
+  <si>
+    <t>First Name: Muhammad
+Last Name: Usman
+Email: test@example.com
+Password: Test@123</t>
+  </si>
+  <si>
+    <t>test@example  /  abc@g.com</t>
+  </si>
+  <si>
+    <t>Numbers/special chars in name
+Te$t</t>
+  </si>
+  <si>
+    <t>First Name: Muhammad
+Last Name: Usman
+Email: test@example.com
+Password: validPassword</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_001</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_002</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_003</t>
+  </si>
+  <si>
+    <t>User is logged out</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_004</t>
+  </si>
+  <si>
+    <t>1. Click on "Continue" button</t>
+  </si>
+  <si>
+    <t>User should be redirected to homepage</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_005</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_006</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_007</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_008</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_009</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_010</t>
+  </si>
+  <si>
+    <t>User is not logged in</t>
+  </si>
+  <si>
+    <t>Verify that "Logout" option is visible after successful login</t>
+  </si>
+  <si>
+    <t>The "Logout" option should be visible in the dropdown menu</t>
+  </si>
+  <si>
+    <t>1. Click on "My Account" dropdown in Header 2. Click on "Logout" option</t>
+  </si>
+  <si>
+    <t>User should be logged out and redirected to logout confirmation page</t>
+  </si>
+  <si>
+    <t>Verify logout confirmation message after successful logout</t>
+  </si>
+  <si>
+    <t>Message: "You have been logged off your account. It is now safe to leave the computer." should be displayed</t>
+  </si>
+  <si>
+    <t>Verify "Continue" button on logout page navigates to homepage</t>
+  </si>
+  <si>
+    <t>User is on logout confirmation page</t>
+  </si>
+  <si>
+    <t>Verify protected pages are not accessible after logout</t>
+  </si>
+  <si>
+    <t>User should be redirected to login page and denied access to account</t>
+  </si>
+  <si>
+    <t>Verify session is destroyed after logout</t>
+  </si>
+  <si>
+    <t>Session data should be cleared after logout</t>
+  </si>
+  <si>
+    <t>Verify browser back does not show protected pages after logout</t>
+  </si>
+  <si>
+    <t>User should not be able to access previous account pages</t>
+  </si>
+  <si>
+    <t>Verify logout behavior across multiple browsers</t>
+  </si>
+  <si>
+    <t>User is logged into two browsers</t>
+  </si>
+  <si>
+    <t>If session is globally tracked, user should be logged out from Browser B too</t>
+  </si>
+  <si>
+    <t>Verify "Logout" option is not visible when not logged in</t>
+  </si>
+  <si>
+    <t>"Logout" option should not be visible in dropdown</t>
+  </si>
+  <si>
+    <t>TC_FP_001</t>
+  </si>
+  <si>
+    <t>User is on Login page</t>
+  </si>
+  <si>
+    <t>Forgot Password page should load</t>
+  </si>
+  <si>
+    <t>TC_FP_002</t>
+  </si>
+  <si>
+    <t>validuser@mail.com</t>
+  </si>
+  <si>
+    <t>User is on Forgot Password page</t>
+  </si>
+  <si>
+    <t>TC_FP_003</t>
+  </si>
+  <si>
+    <t>fakeuser@mail.com</t>
+  </si>
+  <si>
+    <t>TC_FP_004</t>
+  </si>
+  <si>
+    <t>TC_FP_005</t>
+  </si>
+  <si>
+    <t>Placeholder text should be shown</t>
+  </si>
+  <si>
+    <t>TC_FP_006</t>
+  </si>
+  <si>
+    <t>Mandatory field warning appears</t>
+  </si>
+  <si>
+    <t>TC_FP_007</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>Email format validation message shown</t>
+  </si>
+  <si>
+    <t>TC_FP_008</t>
+  </si>
+  <si>
+    <t>User should be redirected to Login page</t>
+  </si>
+  <si>
+    <t>TC_FP_009</t>
+  </si>
+  <si>
+    <t>User is on any page with Right Column</t>
+  </si>
+  <si>
+    <t>Forgot Password page should open</t>
+  </si>
+  <si>
+    <t>TC_FP_010</t>
+  </si>
+  <si>
+    <t>1. Check page breadcrumb navigation</t>
+  </si>
+  <si>
+    <t>Breadcrumb should be visible: Home &gt; Account &gt; Forgot Password</t>
+  </si>
+  <si>
+    <t>TC_FP_011</t>
+  </si>
+  <si>
+    <t>TC_FP_012</t>
+  </si>
+  <si>
+    <t>TC_FP_013</t>
+  </si>
+  <si>
+    <t>User submits valid email</t>
+  </si>
+  <si>
+    <t>TC_FP_014</t>
+  </si>
+  <si>
+    <t>User opens Reset Password page from email</t>
+  </si>
+  <si>
+    <t>UI elements should be aligned and labeled correctly</t>
+  </si>
+  <si>
+    <t>TC_FP_015</t>
+  </si>
+  <si>
+    <t>TS_003
+Logout Functionality</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header 
+3. Click on "Login" from the dropdown 
+4. Enter valid Email and Password 
+5. Click on "Login" button 
+6. Click on "My Account" dropdown</t>
+  </si>
+  <si>
+    <t>Verify that clicking "Logout" option Logout the user successfully</t>
+  </si>
+  <si>
+    <t>1. Click on "My Account" dropdown 
+2. Click on "Logout" option 
+3. Observe the page content</t>
+  </si>
+  <si>
+    <t>1. Open browser
+2. Enter URL: https://demo.opencart.com/index.php?route=account/account 
+3. Press Enter</t>
+  </si>
+  <si>
+    <t>1. Open browser Developer Tools 
+2. Go to Application &gt; Session Storage 
+3. Observe session details</t>
+  </si>
+  <si>
+    <t>1. Click on "My Account" dropdown in Header 
+2. Click on "Login" from the dropdown 
+3. Login successfully 
+4. Logout from account 
+5. Press browser back button</t>
+  </si>
+  <si>
+    <t>1. Login in Browser A with valid credentials 
+2. Login in Browser B with same credentials 
+3. Logout from Browser A 
+4. Refresh account page in Browser B</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header</t>
+  </si>
+  <si>
+    <t>Verify UI of Logout option and Account Logout page</t>
+  </si>
+  <si>
+    <t>1. Navigate to the homepage
+2. Hover over “My Account” in the top menu
+3. Click on “Logout” option
+4. Observe the UI of the 'Account Logout' page</t>
+  </si>
+  <si>
+    <t>“Logout” option should be properly aligned and visible
+‘Account Logout’ page should display heading, breadcrumb, and message clearly with consistent layout</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4. Click “Forgotten Password”</t>
+  </si>
+  <si>
+    <t>Verify user can navigate to Forgot Password page</t>
+  </si>
+  <si>
+    <t>Verify password reset with valid email</t>
+  </si>
+  <si>
+    <t>Verify error with unregistered email</t>
+  </si>
+  <si>
+    <t>Verify empty email field submission</t>
+  </si>
+  <si>
+    <t>Verify placeholder in Email field</t>
+  </si>
+  <si>
+    <t>Verify field is marked mandatory</t>
+  </si>
+  <si>
+    <t>Verify invalid email format input</t>
+  </si>
+  <si>
+    <t>Verify Back button on Forgot Password page</t>
+  </si>
+  <si>
+    <t>Verify navigating from Right Column</t>
+  </si>
+  <si>
+    <t>Verify breadcrumb of the Forgot Password page</t>
+  </si>
+  <si>
+    <t>Verify email with reset instructions is received</t>
+  </si>
+  <si>
+    <t>Verify email reset page UI elements</t>
+  </si>
+  <si>
+    <t>Error: "E-Mail Address was not found in our recods"</t>
+  </si>
+  <si>
+    <t>1. Leave email blank
+2. Click “Continue”</t>
+  </si>
+  <si>
+    <t>1. Leave email blank
+2. Try to submit</t>
+  </si>
+  <si>
+    <t>1. Enter invalid email
+2. Click “Continue”</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4. Click “Forgotten Password”
+5. Click “Back” button</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4. Click “Forgotten Password”
+5. Observe email field</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4.  Click “Forgotten Password” in Right coloumn under My Account</t>
+  </si>
+  <si>
+    <t>Verify reset link cannot be reused after password reset</t>
+  </si>
+  <si>
+    <t>Registered Email: validuser@mail.com</t>
+  </si>
+  <si>
+    <t>Reset password link must be received in email</t>
+  </si>
+  <si>
+    <t>1. Click “Forgotten Password” on Login page
+2. Enter registered email
+3. Click “Continue” to request reset link
+4. Open email and click the reset link
+5. Set new password and confirm it
+6. Submit to complete reset
+7. Click the same reset link again from email</t>
+  </si>
+  <si>
+    <t>System should display "Invalid or expired link" message or redirect to error page</t>
+  </si>
+  <si>
+    <t>1. Navigate to Login page
+2. Click on “Forgotten Password”
+3. Enter registered email: validuser@mail.com
+4. Click “Continue”
+5. Open the email inbox of validuser@mail.com</t>
+  </si>
+  <si>
+    <t>User should receive an email with a reset link and instructions</t>
+  </si>
+  <si>
+    <t>1. Check for labels on "Password" and "Confirm Password" fields
+2. Check for input placeholders
+3. Verify alignment and headings</t>
+  </si>
+  <si>
+    <t>password fields toggle visibility on Reset Password page</t>
+  </si>
+  <si>
+    <t>User must receive a reset password link via email</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link from email
+2. On the “Reset your Password” page, enter text in the “Password” and “Confirm Password” fields
+3. Observe how the input is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters entered in the “Password” and “Confirm Password” fields should appear hidden as ● </t>
+  </si>
+  <si>
+    <t>Validate resetting password without entering values in 'Password' and 'Confirm' fields</t>
+  </si>
+  <si>
+    <t>User must have received a password reset link via email</t>
+  </si>
+  <si>
+    <t>1. Open the password reset email
+2. Click the reset link
+3. On the "Reset your Password" page, leave both fields (Password and Confirm Password) blank
+4. Click the "Continue" button</t>
+  </si>
+  <si>
+    <t>Field-level warning should appear: "Password must be between 4 and 20 characters!" for the Password field</t>
+  </si>
+  <si>
+    <t>A confirmation message should appear stating that reset instructions have been sent to the registered email</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4. Click “Forgotten Password”
+5. Enter unregistered email
+6. Click “Continue”</t>
+  </si>
+  <si>
+    <t>1. Navigate to Homepage 
+2. Click on "My Account" dropdown in Header
+3. Select “Login”
+4. Click “Forgotten Password”
+5. Enter a valid registered email address
+6. Click the “Continue” button</t>
+  </si>
+  <si>
+    <t>TS_004
+Forgot Password</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1860,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1486,12 +1923,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1559,6 +2005,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1601,32 +2077,10 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1650,8 +2104,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1872,7 +2357,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1887,77 +2372,79 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="37">
         <v>45777</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="37"/>
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="C7" s="24"/>
+      <c r="B7" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="34"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
@@ -1990,7 +2477,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2007,7 +2494,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="3">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2024,7 +2511,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2204,7 +2691,7 @@
       <c r="B25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="26" t="s">
         <v>56</v>
       </c>
       <c r="D25" s="16" t="s">
@@ -2221,7 +2708,7 @@
       <c r="B26" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="27" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="18" t="s">
@@ -2494,11 +2981,10 @@
       <c r="E42" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -2519,7 +3005,7 @@
   <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2542,10 +3028,10 @@
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -2575,10 +3061,10 @@
       <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -2608,10 +3094,10 @@
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2641,10 +3127,10 @@
       <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -2674,10 +3160,10 @@
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="45">
         <v>45781</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -2707,10 +3193,10 @@
       <c r="A6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" s="29"/>
+      <c r="B6" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="39"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -2737,9 +3223,9 @@
       <c r="AA6" s="10"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -2766,9 +3252,9 @@
       <c r="AA7" s="10"/>
     </row>
     <row r="8" spans="1:27" s="22" customFormat="1" ht="12.75">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2795,17 +3281,17 @@
       <c r="AA8" s="11"/>
     </row>
     <row r="9" spans="1:27" s="22" customFormat="1" ht="12.75">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -2860,10 +3346,10 @@
     </row>
     <row r="11" spans="1:27" ht="38.25">
       <c r="A11" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>89</v>
@@ -2872,13 +3358,13 @@
         <v>90</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>91</v>
@@ -2909,22 +3395,22 @@
     </row>
     <row r="12" spans="1:27" ht="63.75">
       <c r="A12" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>172</v>
+        <v>346</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>92</v>
@@ -2958,10 +3444,10 @@
     </row>
     <row r="13" spans="1:27" ht="114.75">
       <c r="A13" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>93</v>
@@ -2973,10 +3459,10 @@
         <v>90</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>91</v>
@@ -3007,25 +3493,25 @@
     </row>
     <row r="14" spans="1:27" ht="76.5">
       <c r="A14" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -3050,25 +3536,25 @@
     </row>
     <row r="15" spans="1:27" ht="63.75">
       <c r="A15" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>175</v>
+      <c r="D15" s="28" t="s">
+        <v>341</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>95</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>91</v>
@@ -3099,22 +3585,22 @@
     </row>
     <row r="16" spans="1:27" ht="63.75">
       <c r="A16" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>182</v>
+        <v>345</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>97</v>
@@ -3148,22 +3634,22 @@
     </row>
     <row r="17" spans="1:27" ht="63.75">
       <c r="A17" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>99</v>
@@ -3197,25 +3683,25 @@
     </row>
     <row r="18" spans="1:27" ht="63.75">
       <c r="A18" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>100</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>181</v>
+        <v>344</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>91</v>
@@ -3246,25 +3732,25 @@
     </row>
     <row r="19" spans="1:27" ht="63.75">
       <c r="A19" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>91</v>
@@ -3295,10 +3781,10 @@
     </row>
     <row r="20" spans="1:27" ht="63.75">
       <c r="A20" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>101</v>
@@ -3310,7 +3796,7 @@
         <v>90</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>103</v>
@@ -3344,13 +3830,13 @@
     </row>
     <row r="21" spans="1:27" ht="127.5">
       <c r="A21" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>90</v>
@@ -3359,10 +3845,10 @@
         <v>90</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3387,10 +3873,10 @@
     </row>
     <row r="22" spans="1:27" ht="63.75">
       <c r="A22" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>104</v>
@@ -3402,7 +3888,7 @@
         <v>90</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>106</v>
@@ -3436,10 +3922,10 @@
     </row>
     <row r="23" spans="1:27" ht="38.25">
       <c r="A23" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>107</v>
@@ -3451,7 +3937,7 @@
         <v>90</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>108</v>
@@ -3485,10 +3971,10 @@
     </row>
     <row r="24" spans="1:27" ht="63.75">
       <c r="A24" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>109</v>
@@ -3500,7 +3986,7 @@
         <v>90</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>111</v>
@@ -3534,22 +4020,22 @@
     </row>
     <row r="25" spans="1:27" ht="63.75">
       <c r="A25" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>113</v>
@@ -3583,25 +4069,25 @@
     </row>
     <row r="26" spans="1:27" ht="63.75">
       <c r="A26" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>115</v>
+        <v>342</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>91</v>
@@ -3632,25 +4118,25 @@
     </row>
     <row r="27" spans="1:27" ht="63.75">
       <c r="A27" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>91</v>
@@ -3681,25 +4167,25 @@
     </row>
     <row r="28" spans="1:27" ht="89.25">
       <c r="A28" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>91</v>
@@ -3730,13 +4216,13 @@
     </row>
     <row r="29" spans="1:27" ht="102">
       <c r="A29" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>90</v>
@@ -3745,10 +4231,10 @@
         <v>90</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>91</v>
@@ -3779,25 +4265,25 @@
     </row>
     <row r="30" spans="1:27" ht="89.25">
       <c r="A30" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>240</v>
+        <v>137</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>234</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -3822,25 +4308,25 @@
     </row>
     <row r="31" spans="1:27" ht="102">
       <c r="A31" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -3865,25 +4351,25 @@
     </row>
     <row r="32" spans="1:27" ht="102">
       <c r="A32" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -3908,13 +4394,13 @@
     </row>
     <row r="33" spans="1:27" ht="63.75">
       <c r="A33" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>90</v>
@@ -3923,10 +4409,10 @@
         <v>90</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>91</v>
@@ -3957,25 +4443,25 @@
     </row>
     <row r="34" spans="1:27" ht="38.25">
       <c r="A34" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E34" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="G34" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>91</v>
@@ -4006,25 +4492,25 @@
     </row>
     <row r="35" spans="1:27" ht="127.5">
       <c r="A35" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>91</v>
@@ -4055,25 +4541,25 @@
     </row>
     <row r="36" spans="1:27" ht="114.75">
       <c r="A36" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>91</v>
@@ -4104,25 +4590,25 @@
     </row>
     <row r="37" spans="1:27" ht="51">
       <c r="A37" s="9" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -4147,25 +4633,25 @@
     </row>
     <row r="38" spans="1:27" ht="63.75">
       <c r="A38" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>91</v>
@@ -4196,25 +4682,25 @@
     </row>
     <row r="39" spans="1:27" ht="51">
       <c r="A39" s="9" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E39" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>91</v>
@@ -4245,25 +4731,25 @@
     </row>
     <row r="40" spans="1:27" ht="76.5">
       <c r="A40" s="9" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C40" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>91</v>
@@ -4294,25 +4780,25 @@
     </row>
     <row r="41" spans="1:27" ht="38.25">
       <c r="A41" s="9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E41" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>91</v>
@@ -32347,8 +32833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -32371,10 +32857,10 @@
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -32404,10 +32890,10 @@
       <c r="A2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="48"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -32437,10 +32923,10 @@
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="48"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -32470,10 +32956,10 @@
       <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -32503,10 +32989,10 @@
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="52">
         <v>45781</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -32536,10 +33022,10 @@
       <c r="A6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="52" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" s="53"/>
+      <c r="B6" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="55"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -32566,9 +33052,9 @@
       <c r="AA6" s="10"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -32595,9 +33081,9 @@
       <c r="AA7" s="10"/>
     </row>
     <row r="8" spans="1:27" s="22" customFormat="1">
-      <c r="A8" s="44"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -32624,17 +33110,17 @@
       <c r="AA8" s="11"/>
     </row>
     <row r="9" spans="1:27" s="22" customFormat="1">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -32652,73 +33138,73 @@
       <c r="Z9" s="11"/>
       <c r="AA9" s="11"/>
     </row>
-    <row r="10" spans="1:27" s="46" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="45" t="s">
+    <row r="10" spans="1:27" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="45" t="s">
+      <c r="I10" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="45" t="s">
+      <c r="K10" s="57" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="51">
-      <c r="A11" s="39" t="s">
-        <v>247</v>
+      <c r="A11" s="24" t="s">
+        <v>241</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="24" t="s">
         <v>90</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="H11" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="K11" s="39"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -32737,37 +33223,37 @@
       <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="1:27" ht="76.5">
-      <c r="A12" s="39" t="s">
-        <v>246</v>
+      <c r="A12" s="24" t="s">
+        <v>240</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="E12" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>90</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="H12" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="K12" s="39"/>
+      <c r="K12" s="24"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -32786,60 +33272,60 @@
       <c r="AA12" s="12"/>
     </row>
     <row r="13" spans="1:27" ht="76.5">
-      <c r="A13" s="39" t="s">
-        <v>248</v>
+      <c r="A13" s="24" t="s">
+        <v>242</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="76.5">
-      <c r="A14" s="39" t="s">
-        <v>249</v>
+      <c r="A14" s="24" t="s">
+        <v>243</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G14" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="76.5">
+      <c r="A15" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="76.5">
-      <c r="A15" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>267</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>90</v>
@@ -32848,79 +33334,79 @@
         <v>90</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="89.25">
-      <c r="A16" s="39" t="s">
-        <v>251</v>
+      <c r="A16" s="24" t="s">
+        <v>245</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="89.25">
-      <c r="A17" s="39" t="s">
-        <v>271</v>
+      <c r="A17" s="24" t="s">
+        <v>265</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="76.5">
-      <c r="A18" s="39" t="s">
-        <v>272</v>
+      <c r="A18" s="24" t="s">
+        <v>266</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>292</v>
+        <v>286</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>250</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>91</v>
@@ -32936,26 +33422,26 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="63.75">
-      <c r="A19" s="39" t="s">
-        <v>273</v>
+      <c r="A19" s="24" t="s">
+        <v>267</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>91</v>
@@ -32971,26 +33457,26 @@
       </c>
     </row>
     <row r="20" spans="1:27" ht="89.25">
-      <c r="A20" s="39" t="s">
-        <v>274</v>
+      <c r="A20" s="24" t="s">
+        <v>268</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>91</v>
@@ -33006,26 +33492,26 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="63.75">
-      <c r="A21" s="39" t="s">
-        <v>275</v>
+      <c r="A21" s="24" t="s">
+        <v>269</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>91</v>
@@ -33041,26 +33527,26 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="63.75">
-      <c r="A22" s="39" t="s">
-        <v>276</v>
+      <c r="A22" s="24" t="s">
+        <v>270</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>91</v>
@@ -33076,14 +33562,14 @@
       </c>
     </row>
     <row r="23" spans="1:27" ht="127.5">
-      <c r="A23" s="39" t="s">
-        <v>277</v>
+      <c r="A23" s="24" t="s">
+        <v>271</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>344</v>
+        <v>239</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>329</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>90</v>
@@ -33092,10 +33578,10 @@
         <v>90</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>91</v>
@@ -33111,26 +33597,26 @@
       </c>
     </row>
     <row r="24" spans="1:27" ht="102">
-      <c r="A24" s="39" t="s">
-        <v>278</v>
+      <c r="A24" s="24" t="s">
+        <v>272</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>91</v>
@@ -33145,62 +33631,62 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="76.5">
-      <c r="A25" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="H25" s="9" t="s">
+    <row r="25" spans="1:27" s="22" customFormat="1" ht="89.25">
+      <c r="A25" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="H25" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="K25" s="30" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="89.25">
-      <c r="A26" s="39" t="s">
-        <v>280</v>
+      <c r="A26" s="24" t="s">
+        <v>274</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>91</v>
@@ -33217,25 +33703,25 @@
     </row>
     <row r="27" spans="1:27" ht="127.5">
       <c r="A27" s="9" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>341</v>
+        <v>239</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>326</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>91</v>
@@ -33251,26 +33737,26 @@
       </c>
     </row>
     <row r="28" spans="1:27" ht="63.75">
-      <c r="A28" s="39" t="s">
-        <v>282</v>
+      <c r="A28" s="24" t="s">
+        <v>276</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>91</v>
@@ -33286,26 +33772,26 @@
       </c>
     </row>
     <row r="29" spans="1:27" ht="102">
-      <c r="A29" s="39" t="s">
-        <v>283</v>
+      <c r="A29" s="24" t="s">
+        <v>277</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>91</v>
@@ -33322,25 +33808,25 @@
     </row>
     <row r="30" spans="1:27" ht="114.75">
       <c r="A30" s="9" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9" t="s">
@@ -33354,26 +33840,26 @@
       </c>
     </row>
     <row r="31" spans="1:27" ht="51">
-      <c r="A31" s="39" t="s">
-        <v>285</v>
+      <c r="A31" s="24" t="s">
+        <v>279</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -33396,27 +33882,27 @@
       <c r="Z31" s="13"/>
       <c r="AA31" s="13"/>
     </row>
-    <row r="32" spans="1:27" ht="63.75">
+    <row r="32" spans="1:27" ht="140.25">
       <c r="A32" s="9" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>293</v>
+        <v>90</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>309</v>
+        <v>339</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>302</v>
+        <v>340</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>91</v>
@@ -33432,26 +33918,26 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="25.5">
-      <c r="A33" s="39" t="s">
-        <v>287</v>
+      <c r="A33" s="24" t="s">
+        <v>281</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>91</v>
@@ -33466,19 +33952,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="25.5">
-      <c r="A34" s="39" t="s">
-        <v>288</v>
+    <row r="34" spans="1:11" ht="165.75">
+      <c r="A34" s="24" t="s">
+        <v>282</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
+        <v>239</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>336</v>
+      </c>
       <c r="G34" s="9" t="s">
-        <v>307</v>
+        <v>337</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>91</v>
@@ -33511,24 +34005,1197 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="56" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="31" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="31" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="31" customWidth="1"/>
+    <col min="10" max="10" width="14" style="31" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="31" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="50"/>
+    </row>
+    <row r="2" spans="1:14" ht="15">
+      <c r="A2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="50"/>
+    </row>
+    <row r="3" spans="1:14" ht="30">
+      <c r="A3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" spans="1:14" ht="15">
+      <c r="A4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="50"/>
+    </row>
+    <row r="5" spans="1:14" ht="15">
+      <c r="A5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="52">
+        <v>45781</v>
+      </c>
+      <c r="C5" s="53"/>
+    </row>
+    <row r="6" spans="1:14" ht="15">
+      <c r="A6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+    </row>
+    <row r="10" spans="1:14" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="76.5">
+      <c r="A11" s="59" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="25.5">
+      <c r="A12" s="59" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="38.25">
+      <c r="A13" s="59" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="25.5">
+      <c r="A14" s="59" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="63.75">
+      <c r="A15" s="59" t="s">
+        <v>354</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="38.25">
+      <c r="A16" s="59" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="63.75">
+      <c r="A17" s="59" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>423</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="63.75">
+      <c r="A18" s="59" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="51">
+      <c r="A19" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="25.5">
+      <c r="A20" s="59" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" s="59"/>
+      <c r="D21" s="59"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" s="59"/>
+      <c r="D22" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:N9"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="50"/>
+    </row>
+    <row r="2" spans="1:12" ht="15">
+      <c r="A2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="50"/>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" spans="1:12" ht="15">
+      <c r="A4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="50"/>
+    </row>
+    <row r="5" spans="1:12" ht="15">
+      <c r="A5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="52">
+        <v>45781</v>
+      </c>
+      <c r="C5" s="53"/>
+    </row>
+    <row r="6" spans="1:12" ht="15">
+      <c r="A6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="55"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="65"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+    </row>
+    <row r="10" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="23" customFormat="1" ht="51">
+      <c r="A11" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="23" customFormat="1" ht="76.5">
+      <c r="A12" s="56" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D12" s="58" t="s">
+        <v>384</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>462</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>460</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="23" customFormat="1" ht="76.5">
+      <c r="A13" s="56" t="s">
+        <v>386</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>427</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>387</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>461</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>437</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="23" customFormat="1" ht="25.5">
+      <c r="A14" s="56" t="s">
+        <v>388</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>437</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="23" customFormat="1" ht="63.75">
+      <c r="A15" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>442</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="23" customFormat="1" ht="25.5">
+      <c r="A16" s="56" t="s">
+        <v>391</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>430</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="23" customFormat="1" ht="25.5">
+      <c r="A17" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>440</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="23" customFormat="1" ht="63.75">
+      <c r="A18" s="56" t="s">
+        <v>396</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>432</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>441</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="23" customFormat="1" ht="63.75">
+      <c r="A19" s="56" t="s">
+        <v>398</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>443</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="23" customFormat="1" ht="25.5">
+      <c r="A20" s="56" t="s">
+        <v>401</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>434</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="23" customFormat="1" ht="63.75">
+      <c r="A21" s="56" t="s">
+        <v>404</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C21" t="s">
+        <v>456</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>458</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>459</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="23" customFormat="1" ht="89.25">
+      <c r="A22" s="56" t="s">
+        <v>405</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>444</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>446</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>447</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>448</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="23" customFormat="1" ht="63.75">
+      <c r="A23" s="56" t="s">
+        <v>406</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>435</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="23" customFormat="1" ht="51">
+      <c r="A24" s="56" t="s">
+        <v>408</v>
+      </c>
+      <c r="B24" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>436</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>409</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="23" customFormat="1" ht="51">
+      <c r="A25" s="56" t="s">
+        <v>411</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>463</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>453</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>454</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>455</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="23" customFormat="1">
+      <c r="A26" s="67"/>
+      <c r="B26" s="67"/>
+    </row>
+    <row r="27" spans="1:11" s="23" customFormat="1">
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="64"/>
+      <c r="B28" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>